<commit_message>
updated end points for basic crud on family member
</commit_message>
<xml_diff>
--- a/notes/http methods.xlsx
+++ b/notes/http methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\github\hdb_assignment\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABAE36-1019-459D-9DD9-92C81E5B60CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B3570-21BE-457F-B232-27CBADACCB4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13032" yWindow="2736" windowWidth="10896" windowHeight="8964" xr2:uid="{AA613092-2076-41D8-B0A8-1860B215704A}"/>
+    <workbookView xWindow="10260" yWindow="2244" windowWidth="10896" windowHeight="8964" xr2:uid="{AA613092-2076-41D8-B0A8-1860B215704A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>HTTP method</t>
   </si>
@@ -66,21 +66,9 @@
     <t>Delete a household</t>
   </si>
   <si>
-    <t xml:space="preserve">DELETE </t>
-  </si>
-  <si>
     <t>/household/family/delete</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>/household/listTypes</t>
-  </si>
-  <si>
-    <t>Read a list of householdTypes</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -88,14 +76,55 @@
   </si>
   <si>
     <t>/household/family/update</t>
+  </si>
+  <si>
+    <t>HouseholdRestcontroller</t>
+  </si>
+  <si>
+    <t>/household/update</t>
+  </si>
+  <si>
+    <t>Update a household</t>
+  </si>
+  <si>
+    <t>FamilyMemberRestcontroller</t>
+  </si>
+  <si>
+    <t>/household/family/list</t>
+  </si>
+  <si>
+    <t>/household/family/list/{familyMemberId}</t>
+  </si>
+  <si>
+    <t>Read a list of family members</t>
+  </si>
+  <si>
+    <t>Read a single family member</t>
+  </si>
+  <si>
+    <t>Create a new family member</t>
+  </si>
+  <si>
+    <t>Update a family member</t>
+  </si>
+  <si>
+    <t>Delete a family member</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,8 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E771B4-A52F-47DD-A086-C48761CA1E73}">
-  <dimension ref="A2:I10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,15 +480,20 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -468,11 +503,8 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -482,33 +514,30 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -519,31 +548,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+      <c r="F15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new endpoint for list of schemes
</commit_message>
<xml_diff>
--- a/notes/http methods.xlsx
+++ b/notes/http methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\github\hdb_assignment\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B3570-21BE-457F-B232-27CBADACCB4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F900F48-DA0E-4CCD-A15E-B926CB7FFED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="2244" windowWidth="10896" windowHeight="8964" xr2:uid="{AA613092-2076-41D8-B0A8-1860B215704A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>HTTP method</t>
   </si>
@@ -109,6 +109,48 @@
   </si>
   <si>
     <t>Delete a family member</t>
+  </si>
+  <si>
+    <t>Optional Param</t>
+  </si>
+  <si>
+    <t>householdSize, total_income</t>
+  </si>
+  <si>
+    <t>/household/family/list/student?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>/household/family/list/family?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>Student Encouragement Bonus List</t>
+  </si>
+  <si>
+    <t>Family Togetherness Scheme List</t>
+  </si>
+  <si>
+    <t>/household/family/list/elder?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>/household/family/list/baby?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>/household/family/list/yolo?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>Baby Sunshine Grant List</t>
+  </si>
+  <si>
+    <t>Elder Bonus List</t>
+  </si>
+  <si>
+    <t>Yolo Gst Grant List</t>
+  </si>
+  <si>
+    <t>/household/family/list/schemes?householdSize=2&amp;totalIncome=3000</t>
+  </si>
+  <si>
+    <t>Get all grants</t>
   </si>
 </sst>
 </file>
@@ -469,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E771B4-A52F-47DD-A086-C48761CA1E73}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,12 +522,12 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -504,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -515,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -526,7 +568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -537,7 +579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -548,12 +590,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -572,7 +614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -583,7 +625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -594,7 +636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -605,7 +647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -616,8 +658,108 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{A522CD5B-9857-45A3-B158-1CF45135C92C}"/>
+    <hyperlink ref="B18" r:id="rId2" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{AB0A1DBF-46B7-42E2-87A3-1DEC7D0B9CD1}"/>
+    <hyperlink ref="B19" r:id="rId3" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{67928764-927D-4441-9188-B4DCFC2436C8}"/>
+    <hyperlink ref="B20" r:id="rId4" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{FA114EDF-FF84-4269-8EE1-778AC4F63B67}"/>
+    <hyperlink ref="B21" r:id="rId5" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{3BFA6E38-542B-48F5-B6EA-A79543DCA2C1}"/>
+    <hyperlink ref="B23" r:id="rId6" display="http://localhost:8080/household/family/list/studentEncouragement?householdSize=2&amp;total_income=3000" xr:uid="{1BEAE1B8-DBE2-4E78-9735-75D8CFC50228}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated endpoint for scheme type search
</commit_message>
<xml_diff>
--- a/notes/http methods.xlsx
+++ b/notes/http methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\github\hdb_assignment\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F900F48-DA0E-4CCD-A15E-B926CB7FFED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03502278-B89A-4893-A1E0-DA33C8A5C652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="2244" windowWidth="10896" windowHeight="8964" xr2:uid="{AA613092-2076-41D8-B0A8-1860B215704A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>HTTP method</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Get all grants</t>
+  </si>
+  <si>
+    <t>/household/family/list/scheme?type=yolo,student&amp;householdSize=8&amp;totalIncome=300000</t>
+  </si>
+  <si>
+    <t>Get grant or grants</t>
+  </si>
+  <si>
+    <t>householdSize, total_income, type={student, family, elder, baby, yolo}</t>
   </si>
 </sst>
 </file>
@@ -511,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E771B4-A52F-47DD-A086-C48761CA1E73}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,6 +757,20 @@
       </c>
       <c r="M23" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>